<commit_message>
0820 home nodejs E-class
</commit_message>
<xml_diff>
--- a/수강률.xlsx
+++ b/수강률.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bizworks\Biz_NodeJs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bizworks\Nodejs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="90">
   <si>
     <t>강의</t>
   </si>
@@ -304,7 +304,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -639,15 +639,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:I170"/>
+  <dimension ref="B3:I148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="K147" sqref="K147"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="3" max="3" width="9" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="11.625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="13.75" bestFit="1" customWidth="1"/>
   </cols>
@@ -687,19 +687,19 @@
       </c>
       <c r="F4" t="str">
         <f>SUM(C4:C170)&amp;"분"</f>
-        <v>1653분</v>
+        <v>1469분</v>
       </c>
       <c r="G4" t="str">
         <f>SUMIF(D4:D170,"Y",C4:C170)&amp;"분"</f>
-        <v>206분</v>
+        <v>265분</v>
       </c>
       <c r="H4" t="str">
         <f>SUMIF(D4:D170,"N",C4:C170)&amp;"분"</f>
-        <v>1447분</v>
+        <v>1204분</v>
       </c>
       <c r="I4" s="1">
         <f>SUMIF(D4:D170,"Y",C4:C170)/SUM(C4:C170)</f>
-        <v>0.12462189957652753</v>
+        <v>0.18039482641252552</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
@@ -922,7 +922,7 @@
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
@@ -933,7 +933,7 @@
         <v>11</v>
       </c>
       <c r="D25" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
@@ -944,7 +944,7 @@
         <v>13</v>
       </c>
       <c r="D26" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
@@ -955,7 +955,7 @@
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
@@ -966,7 +966,7 @@
         <v>11</v>
       </c>
       <c r="D28" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.3">
@@ -977,7 +977,7 @@
         <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.3">
@@ -988,7 +988,7 @@
         <v>10</v>
       </c>
       <c r="D30" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
@@ -2286,248 +2286,6 @@
         <v>28</v>
       </c>
       <c r="D148" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="149" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B149" t="s">
-        <v>3</v>
-      </c>
-      <c r="C149">
-        <v>2</v>
-      </c>
-      <c r="D149" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="150" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B150" t="s">
-        <v>5</v>
-      </c>
-      <c r="C150">
-        <v>9</v>
-      </c>
-      <c r="D150" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="151" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B151" t="s">
-        <v>6</v>
-      </c>
-      <c r="C151">
-        <v>5</v>
-      </c>
-      <c r="D151" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="152" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B152" t="s">
-        <v>7</v>
-      </c>
-      <c r="C152">
-        <v>4</v>
-      </c>
-      <c r="D152" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="153" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B153" t="s">
-        <v>9</v>
-      </c>
-      <c r="C153">
-        <v>8</v>
-      </c>
-      <c r="D153" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="154" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B154" t="s">
-        <v>10</v>
-      </c>
-      <c r="C154">
-        <v>11</v>
-      </c>
-      <c r="D154" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="155" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B155" t="s">
-        <v>11</v>
-      </c>
-      <c r="C155">
-        <v>8</v>
-      </c>
-      <c r="D155" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="156" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B156" t="s">
-        <v>12</v>
-      </c>
-      <c r="C156">
-        <v>12</v>
-      </c>
-      <c r="D156" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="157" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B157" t="s">
-        <v>13</v>
-      </c>
-      <c r="C157">
-        <v>9</v>
-      </c>
-      <c r="D157" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="158" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B158" t="s">
-        <v>14</v>
-      </c>
-      <c r="C158">
-        <v>8</v>
-      </c>
-      <c r="D158" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="159" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B159" t="s">
-        <v>15</v>
-      </c>
-      <c r="C159">
-        <v>22</v>
-      </c>
-      <c r="D159" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="160" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B160" t="s">
-        <v>16</v>
-      </c>
-      <c r="C160">
-        <v>8</v>
-      </c>
-      <c r="D160" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="161" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B161" t="s">
-        <v>17</v>
-      </c>
-      <c r="C161">
-        <v>8</v>
-      </c>
-      <c r="D161" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="162" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B162" t="s">
-        <v>18</v>
-      </c>
-      <c r="C162">
-        <v>8</v>
-      </c>
-      <c r="D162" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="163" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B163" t="s">
-        <v>19</v>
-      </c>
-      <c r="C163">
-        <v>9</v>
-      </c>
-      <c r="D163" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="164" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B164" t="s">
-        <v>20</v>
-      </c>
-      <c r="C164">
-        <v>9</v>
-      </c>
-      <c r="D164" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="165" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B165" t="s">
-        <v>21</v>
-      </c>
-      <c r="C165">
-        <v>9</v>
-      </c>
-      <c r="D165" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="166" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B166" t="s">
-        <v>22</v>
-      </c>
-      <c r="C166">
-        <v>13</v>
-      </c>
-      <c r="D166" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="167" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B167" t="s">
-        <v>23</v>
-      </c>
-      <c r="C167">
-        <v>11</v>
-      </c>
-      <c r="D167" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="168" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B168" t="s">
-        <v>24</v>
-      </c>
-      <c r="C168">
-        <v>3</v>
-      </c>
-      <c r="D168" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="169" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B169" t="s">
-        <v>25</v>
-      </c>
-      <c r="C169">
-        <v>4</v>
-      </c>
-      <c r="D169" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="170" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B170" t="s">
-        <v>26</v>
-      </c>
-      <c r="C170">
-        <v>4</v>
-      </c>
-      <c r="D170" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
0821 home nodejs e-class
</commit_message>
<xml_diff>
--- a/수강률.xlsx
+++ b/수강률.xlsx
@@ -646,7 +646,7 @@
   <dimension ref="B3:I148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -695,15 +695,15 @@
       </c>
       <c r="G4" t="str">
         <f>SUMIF(D4:D170,"Y",C4:C170)&amp;"분"</f>
-        <v>357분</v>
+        <v>421분</v>
       </c>
       <c r="H4" t="str">
         <f>SUMIF(D4:D170,"N",C4:C170)&amp;"분"</f>
-        <v>1112분</v>
+        <v>1048분</v>
       </c>
       <c r="I4" s="1">
         <f>SUMIF(D4:D170,"Y",C4:C170)/SUM(C4:C170)</f>
-        <v>0.24302246426140231</v>
+        <v>0.28658951667801225</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
@@ -1105,7 +1105,7 @@
         <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
@@ -1116,7 +1116,7 @@
         <v>13</v>
       </c>
       <c r="D41" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
@@ -1127,7 +1127,7 @@
         <v>9</v>
       </c>
       <c r="D42" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
@@ -1138,7 +1138,7 @@
         <v>13</v>
       </c>
       <c r="D43" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
@@ -1149,7 +1149,7 @@
         <v>10</v>
       </c>
       <c r="D44" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
@@ -1160,7 +1160,7 @@
         <v>4</v>
       </c>
       <c r="D45" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
@@ -1171,7 +1171,7 @@
         <v>8</v>
       </c>
       <c r="D46" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
0823 home nodejs express, MySQL 간단한 list 만들기
</commit_message>
<xml_diff>
--- a/수강률.xlsx
+++ b/수강률.xlsx
@@ -645,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I148"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -695,15 +695,15 @@
       </c>
       <c r="G4" t="str">
         <f>SUMIF(D4:D170,"Y",C4:C170)&amp;"분"</f>
-        <v>421분</v>
+        <v>649분</v>
       </c>
       <c r="H4" t="str">
         <f>SUMIF(D4:D170,"N",C4:C170)&amp;"분"</f>
-        <v>1048분</v>
+        <v>820분</v>
       </c>
       <c r="I4" s="1">
         <f>SUMIF(D4:D170,"Y",C4:C170)/SUM(C4:C170)</f>
-        <v>0.28658951667801225</v>
+        <v>0.44179714091218514</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
@@ -1182,7 +1182,7 @@
         <v>6</v>
       </c>
       <c r="D47" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.3">
@@ -1193,7 +1193,7 @@
         <v>8</v>
       </c>
       <c r="D48" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.3">
@@ -1204,7 +1204,7 @@
         <v>8</v>
       </c>
       <c r="D49" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
@@ -1215,7 +1215,7 @@
         <v>9</v>
       </c>
       <c r="D50" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.3">
@@ -1226,7 +1226,7 @@
         <v>8</v>
       </c>
       <c r="D51" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.3">
@@ -1237,7 +1237,7 @@
         <v>10</v>
       </c>
       <c r="D52" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.3">
@@ -1248,7 +1248,7 @@
         <v>7</v>
       </c>
       <c r="D53" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.3">
@@ -1259,7 +1259,7 @@
         <v>16</v>
       </c>
       <c r="D54" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.3">
@@ -1270,7 +1270,7 @@
         <v>12</v>
       </c>
       <c r="D55" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.3">
@@ -1281,7 +1281,7 @@
         <v>10</v>
       </c>
       <c r="D56" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.3">
@@ -1292,7 +1292,7 @@
         <v>13</v>
       </c>
       <c r="D57" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.3">
@@ -1303,7 +1303,7 @@
         <v>14</v>
       </c>
       <c r="D58" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.3">
@@ -1314,7 +1314,7 @@
         <v>13</v>
       </c>
       <c r="D59" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.3">
@@ -1325,7 +1325,7 @@
         <v>8</v>
       </c>
       <c r="D60" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.3">
@@ -1336,7 +1336,7 @@
         <v>8</v>
       </c>
       <c r="D61" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.3">
@@ -1347,7 +1347,7 @@
         <v>12</v>
       </c>
       <c r="D62" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.3">
@@ -1358,7 +1358,7 @@
         <v>8</v>
       </c>
       <c r="D63" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.3">
@@ -1369,7 +1369,7 @@
         <v>11</v>
       </c>
       <c r="D64" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.3">
@@ -1380,7 +1380,7 @@
         <v>13</v>
       </c>
       <c r="D65" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.3">
@@ -1391,7 +1391,7 @@
         <v>10</v>
       </c>
       <c r="D66" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.3">
@@ -1402,7 +1402,7 @@
         <v>13</v>
       </c>
       <c r="D67" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.3">
@@ -1413,7 +1413,7 @@
         <v>11</v>
       </c>
       <c r="D68" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.3">

</xml_diff>